<commit_message>
updated to include detection limit information
</commit_message>
<xml_diff>
--- a/data/JMHnewMungedDat/maximum detection limits.xlsx
+++ b/data/JMHnewMungedDat/maximum detection limits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MAR Project New 2020\Raw Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hood.211/Dropbox/JMH_dropbox/stephanson2/projects/6_Research/IrenasPaper/bgc_meta/data/JMHnewMungedDat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BE2BA1-719E-48CC-A161-BB01B53FEDAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EE693B-F631-5B46-8317-0BFCD177AF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8728EA87-E39C-408C-9DA9-45602A0991CC}"/>
+    <workbookView xWindow="55660" yWindow="13440" windowWidth="20740" windowHeight="11160" xr2:uid="{8728EA87-E39C-408C-9DA9-45602A0991CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Ca mgL</t>
   </si>
@@ -87,6 +87,42 @@
   </si>
   <si>
     <t>TP/TDP/PO4-P mgL</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>SiteCode</t>
+  </si>
+  <si>
+    <t>BBWM</t>
+  </si>
+  <si>
+    <t>DOR</t>
+  </si>
+  <si>
+    <t>HBEF</t>
+  </si>
+  <si>
+    <t>HJA</t>
+  </si>
+  <si>
+    <t>MEF</t>
+  </si>
+  <si>
+    <t>SLP</t>
+  </si>
+  <si>
+    <t>TLW</t>
+  </si>
+  <si>
+    <t>COW</t>
+  </si>
+  <si>
+    <t>LUQ</t>
+  </si>
+  <si>
+    <t>SAN</t>
   </si>
 </sst>
 </file>
@@ -444,288 +480,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2D4969-1166-4102-A923-E22056B9F411}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
         <v>0.01</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.05</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.4E-3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
         <v>0.12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2E-3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>6.8400000000000002E-2</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
         <v>0.1</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.3</v>
-      </c>
-      <c r="D4">
-        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G4">
         <v>3.2000000000000003E-4</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>0.02</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.51600000000000001</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.1200000000000001E-3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.34</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
         <v>0.06</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.05</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.01</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1E-3</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2E-3</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>0.1</v>
+      <c r="B8" t="s">
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0.1</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.01</v>
+      <c r="D8">
+        <v>0.1</v>
       </c>
       <c r="E8" s="2">
         <v>0.01</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G8">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
         <v>0.05</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9">
         <v>0.05</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
         <v>0.05</v>
-      </c>
-      <c r="C10">
-        <v>0.1</v>
       </c>
       <c r="D10">
         <v>0.1</v>
       </c>
       <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
         <v>0.2</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.1</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.376</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.4</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.01</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.04</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1E-3</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>